<commit_message>
Merged PR 1734: Task 335717: Багфикс TLC
Task 335717: Багфикс TLC
</commit_message>
<xml_diff>
--- a/Module.Frontend.TPM/Templates/TLCClosedTemplate.xlsx
+++ b/Module.Frontend.TPM/Templates/TLCClosedTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Windows\Temp\TPM\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E83062-3B64-42BC-B0E4-FA2DEF2950E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5631B51-4713-4BF8-B59F-D4766EAB18D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Promo Type</t>
   </si>
@@ -411,51 +411,6 @@
   </si>
   <si>
     <t>InOut Promo</t>
-  </si>
-  <si>
-    <t>Catsan Litter</t>
-  </si>
-  <si>
-    <t>Cesar Pouch</t>
-  </si>
-  <si>
-    <t>10litre</t>
-  </si>
-  <si>
-    <t>2.5litre</t>
-  </si>
-  <si>
-    <t>2piece</t>
-  </si>
-  <si>
-    <t>5litre</t>
-  </si>
-  <si>
-    <t>100g</t>
-  </si>
-  <si>
-    <t>2.38kg</t>
-  </si>
-  <si>
-    <t>3.75kg</t>
-  </si>
-  <si>
-    <t>500g</t>
-  </si>
-  <si>
-    <t>80g</t>
-  </si>
-  <si>
-    <t>85g</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>TPR</t>
-  </si>
-  <si>
-    <t>VP</t>
   </si>
 </sst>
 </file>
@@ -6715,99 +6670,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E49EAC7-9F4D-46B4-B4A5-AFAF69F8538B}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6816,26 +6684,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC80930-7F4F-4A05-A0B9-C5579139E38B}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>